<commit_message>
Maybe end? idk... im tired.
</commit_message>
<xml_diff>
--- a/data/xlsx/Technology_List_Land.xlsx
+++ b/data/xlsx/Technology_List_Land.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/User/Desktop/clews-horizon-visualizer/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61084703-23BE-5842-8329-8A8CF73F8315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94571C7-503B-4F4A-90E2-2A0FC5FB224A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21180" yWindow="6400" windowWidth="27240" windowHeight="16440" xr2:uid="{F08CDD2F-48E4-E24B-B1FD-96D4AE9CFB50}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="27140" xr2:uid="{F08CDD2F-48E4-E24B-B1FD-96D4AE9CFB50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -224,9 +224,6 @@
     <t>BRL</t>
   </si>
   <si>
-    <t>IMCBAR</t>
-  </si>
-  <si>
     <t>SUN</t>
   </si>
   <si>
@@ -296,9 +293,6 @@
     <t>EULBAR</t>
   </si>
   <si>
-    <t>EXCBAR</t>
-  </si>
-  <si>
     <t>EULSUN</t>
   </si>
   <si>
@@ -606,13 +600,19 @@
   </si>
   <si>
     <t>Backstop for Other crops production</t>
+  </si>
+  <si>
+    <t>IMCBRL</t>
+  </si>
+  <si>
+    <t>EXCBRL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -634,12 +634,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -766,10 +760,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1092,7 +1082,7 @@
   <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1321,7 +1311,7 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>35</v>
+        <v>161</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="4" t="s">
@@ -1361,7 +1351,7 @@
         <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1370,7 +1360,7 @@
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="4" t="s">
@@ -1383,7 +1373,7 @@
         <v>31</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O6" s="4">
         <v>0</v>
@@ -1410,7 +1400,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -1419,7 +1409,7 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="4" t="s">
@@ -1432,7 +1422,7 @@
         <v>31</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O7" s="4">
         <v>0</v>
@@ -1459,7 +1449,7 @@
         <v>27</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1468,7 +1458,7 @@
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="4" t="s">
@@ -1481,7 +1471,7 @@
         <v>31</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O8" s="4">
         <v>0</v>
@@ -1508,7 +1498,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1517,7 +1507,7 @@
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="4" t="s">
@@ -1530,7 +1520,7 @@
         <v>31</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O9" s="4">
         <v>0</v>
@@ -1557,7 +1547,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1566,7 +1556,7 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="4" t="s">
@@ -1579,7 +1569,7 @@
         <v>31</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O10" s="4">
         <v>0</v>
@@ -1606,7 +1596,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1615,7 +1605,7 @@
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="4" t="s">
@@ -1628,7 +1618,7 @@
         <v>31</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O11" s="4">
         <v>0</v>
@@ -1655,7 +1645,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -1664,7 +1654,7 @@
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="7" t="s">
@@ -1677,7 +1667,7 @@
         <v>31</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O12" s="7">
         <v>0</v>
@@ -1704,7 +1694,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1713,7 +1703,7 @@
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J13" s="5"/>
       <c r="K13" s="4" t="s">
@@ -1726,7 +1716,7 @@
         <v>31</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O13" s="4">
         <v>0</v>
@@ -1750,7 +1740,7 @@
         <v>18</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>28</v>
@@ -1758,11 +1748,11 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="4" t="s">
@@ -1772,7 +1762,7 @@
         <v>24</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N14" s="4" t="s">
         <v>28</v>
@@ -1799,7 +1789,7 @@
         <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>32</v>
@@ -1807,11 +1797,11 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="4" t="s">
@@ -1821,7 +1811,7 @@
         <v>24</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>32</v>
@@ -1848,7 +1838,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>34</v>
@@ -1856,11 +1846,11 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4" t="s">
-        <v>59</v>
+        <v>162</v>
       </c>
       <c r="J16" s="5"/>
       <c r="K16" s="4" t="s">
@@ -1870,7 +1860,7 @@
         <v>24</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>34</v>
@@ -1897,19 +1887,19 @@
         <v>18</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J17" s="5"/>
       <c r="K17" s="4" t="s">
@@ -1919,10 +1909,10 @@
         <v>24</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O17" s="4">
         <v>0</v>
@@ -1946,19 +1936,19 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J18" s="5"/>
       <c r="K18" s="4" t="s">
@@ -1968,10 +1958,10 @@
         <v>24</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O18" s="4">
         <v>0</v>
@@ -1995,19 +1985,19 @@
         <v>18</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="4" t="s">
@@ -2017,10 +2007,10 @@
         <v>24</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O19" s="4">
         <v>0</v>
@@ -2044,19 +2034,19 @@
         <v>18</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="4" t="s">
@@ -2066,10 +2056,10 @@
         <v>24</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O20" s="4">
         <v>0</v>
@@ -2093,19 +2083,19 @@
         <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="4" t="s">
@@ -2115,10 +2105,10 @@
         <v>24</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O21" s="4">
         <v>0</v>
@@ -2142,19 +2132,19 @@
         <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J22" s="5"/>
       <c r="K22" s="4" t="s">
@@ -2164,10 +2154,10 @@
         <v>24</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O22" s="4">
         <v>0</v>
@@ -2191,19 +2181,19 @@
         <v>18</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J23" s="5"/>
       <c r="K23" s="4" t="s">
@@ -2213,10 +2203,10 @@
         <v>24</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O23" s="4">
         <v>0</v>
@@ -2240,19 +2230,19 @@
         <v>18</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J24" s="5"/>
       <c r="K24" s="4" t="s">
@@ -2262,10 +2252,10 @@
         <v>24</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O24" s="4">
         <v>0</v>
@@ -2289,19 +2279,19 @@
         <v>18</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J25" s="5"/>
       <c r="K25" s="4" t="s">
@@ -2317,10 +2307,10 @@
         <v>28</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q25" s="4">
         <v>0</v>
@@ -2338,19 +2328,19 @@
         <v>18</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J26" s="5"/>
       <c r="K26" s="4" t="s">
@@ -2366,10 +2356,10 @@
         <v>32</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q26" s="4">
         <v>0</v>
@@ -2387,19 +2377,19 @@
         <v>18</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J27" s="5"/>
       <c r="K27" s="4" t="s">
@@ -2415,10 +2405,10 @@
         <v>34</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q27" s="4">
         <v>0</v>
@@ -2436,19 +2426,19 @@
         <v>18</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J28" s="5"/>
       <c r="K28" s="4" t="s">
@@ -2461,13 +2451,13 @@
         <v>25</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q28" s="4">
         <v>0</v>
@@ -2485,19 +2475,19 @@
         <v>18</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="4" t="s">
@@ -2510,13 +2500,13 @@
         <v>25</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q29" s="4">
         <v>0</v>
@@ -2534,19 +2524,19 @@
         <v>18</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J30" s="5"/>
       <c r="K30" s="4" t="s">
@@ -2559,13 +2549,13 @@
         <v>25</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q30" s="4">
         <v>0</v>
@@ -2583,19 +2573,19 @@
         <v>18</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="4" t="s">
@@ -2608,13 +2598,13 @@
         <v>25</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q31" s="4">
         <v>0</v>
@@ -2632,19 +2622,19 @@
         <v>18</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="4" t="s">
@@ -2657,13 +2647,13 @@
         <v>25</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q32" s="4">
         <v>0</v>
@@ -2681,19 +2671,19 @@
         <v>18</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="4" t="s">
@@ -2706,13 +2696,13 @@
         <v>25</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q33" s="4">
         <v>0</v>
@@ -2730,19 +2720,19 @@
         <v>18</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="4" t="s">
@@ -2755,13 +2745,13 @@
         <v>25</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q34" s="4">
         <v>0</v>
@@ -2779,19 +2769,19 @@
         <v>18</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="4" t="s">
@@ -2804,13 +2794,13 @@
         <v>25</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O35" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q35" s="4">
         <v>0</v>
@@ -2828,19 +2818,19 @@
         <v>18</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="4" t="s">
@@ -2856,10 +2846,10 @@
         <v>28</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P36" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q36" s="4">
         <v>0</v>
@@ -2877,19 +2867,19 @@
         <v>18</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J37" s="5"/>
       <c r="K37" s="4" t="s">
@@ -2905,10 +2895,10 @@
         <v>32</v>
       </c>
       <c r="O37" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P37" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q37" s="4">
         <v>0</v>
@@ -2926,19 +2916,19 @@
         <v>18</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="8" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J38" s="5"/>
       <c r="K38" s="4" t="s">
@@ -2954,10 +2944,10 @@
         <v>34</v>
       </c>
       <c r="O38" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P38" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q38" s="4">
         <v>0</v>
@@ -2975,19 +2965,19 @@
         <v>18</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J39" s="5"/>
       <c r="K39" s="4" t="s">
@@ -3000,13 +2990,13 @@
         <v>25</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P39" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q39" s="4">
         <v>0</v>
@@ -3024,19 +3014,19 @@
         <v>18</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="4" t="s">
@@ -3049,13 +3039,13 @@
         <v>25</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O40" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P40" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q40" s="4">
         <v>0</v>
@@ -3073,19 +3063,19 @@
         <v>18</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J41" s="5"/>
       <c r="K41" s="4" t="s">
@@ -3098,13 +3088,13 @@
         <v>25</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O41" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P41" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q41" s="4">
         <v>0</v>
@@ -3122,19 +3112,19 @@
         <v>18</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J42" s="5"/>
       <c r="K42" s="4" t="s">
@@ -3147,13 +3137,13 @@
         <v>25</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P42" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q42" s="4">
         <v>0</v>
@@ -3171,19 +3161,19 @@
         <v>18</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J43" s="5"/>
       <c r="K43" s="4" t="s">
@@ -3196,13 +3186,13 @@
         <v>25</v>
       </c>
       <c r="N43" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O43" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P43" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q43" s="4">
         <v>0</v>
@@ -3220,19 +3210,19 @@
         <v>18</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="4" t="s">
@@ -3245,13 +3235,13 @@
         <v>25</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O44" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P44" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q44" s="4">
         <v>0</v>
@@ -3269,19 +3259,19 @@
         <v>18</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="4" t="s">
@@ -3294,13 +3284,13 @@
         <v>25</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O45" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P45" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q45" s="4">
         <v>0</v>
@@ -3318,19 +3308,19 @@
         <v>18</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="4" t="s">
@@ -3343,13 +3333,13 @@
         <v>25</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O46" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P46" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q46" s="4">
         <v>0</v>
@@ -3367,19 +3357,19 @@
         <v>18</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J47" s="5"/>
       <c r="K47" s="4" t="s">
@@ -3398,7 +3388,7 @@
         <v>24</v>
       </c>
       <c r="P47" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q47" s="4">
         <v>0</v>
@@ -3416,19 +3406,19 @@
         <v>18</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J48" s="5"/>
       <c r="K48" s="4" t="s">
@@ -3447,7 +3437,7 @@
         <v>24</v>
       </c>
       <c r="P48" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q48" s="4">
         <v>0</v>
@@ -3465,19 +3455,19 @@
         <v>18</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J49" s="5"/>
       <c r="K49" s="4" t="s">
@@ -3496,7 +3486,7 @@
         <v>24</v>
       </c>
       <c r="P49" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q49" s="4">
         <v>0</v>
@@ -3514,19 +3504,19 @@
         <v>18</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J50" s="5"/>
       <c r="K50" s="4" t="s">
@@ -3539,13 +3529,13 @@
         <v>25</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O50" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P50" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q50" s="4">
         <v>0</v>
@@ -3563,19 +3553,19 @@
         <v>18</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J51" s="5"/>
       <c r="K51" s="4" t="s">
@@ -3588,13 +3578,13 @@
         <v>25</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O51" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P51" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q51" s="4">
         <v>0</v>
@@ -3612,19 +3602,19 @@
         <v>18</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H52" s="4"/>
       <c r="I52" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J52" s="5"/>
       <c r="K52" s="4" t="s">
@@ -3637,13 +3627,13 @@
         <v>25</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O52" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P52" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q52" s="4">
         <v>0</v>
@@ -3661,19 +3651,19 @@
         <v>18</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H53" s="4"/>
       <c r="I53" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J53" s="5"/>
       <c r="K53" s="4" t="s">
@@ -3686,13 +3676,13 @@
         <v>25</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O53" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P53" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q53" s="4">
         <v>0</v>
@@ -3710,19 +3700,19 @@
         <v>18</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H54" s="4"/>
       <c r="I54" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J54" s="5"/>
       <c r="K54" s="4" t="s">
@@ -3735,13 +3725,13 @@
         <v>25</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O54" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P54" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q54" s="4">
         <v>0</v>
@@ -3759,19 +3749,19 @@
         <v>18</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J55" s="5"/>
       <c r="K55" s="4" t="s">
@@ -3784,13 +3774,13 @@
         <v>25</v>
       </c>
       <c r="N55" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O55" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P55" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q55" s="4">
         <v>0</v>
@@ -3808,19 +3798,19 @@
         <v>18</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="4" t="s">
@@ -3833,13 +3823,13 @@
         <v>25</v>
       </c>
       <c r="N56" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O56" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P56" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q56" s="4">
         <v>0</v>
@@ -3857,19 +3847,19 @@
         <v>18</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J57" s="5"/>
       <c r="K57" s="4" t="s">
@@ -3882,13 +3872,13 @@
         <v>25</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O57" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P57" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="Q57" s="4">
         <v>0</v>
@@ -3906,19 +3896,19 @@
         <v>18</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H58" s="4"/>
       <c r="I58" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J58" s="5"/>
       <c r="K58" s="4" t="s">
@@ -3937,7 +3927,7 @@
         <v>24</v>
       </c>
       <c r="P58" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q58" s="4">
         <v>0</v>
@@ -3955,19 +3945,19 @@
         <v>18</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J59" s="5"/>
       <c r="K59" s="4" t="s">
@@ -3986,7 +3976,7 @@
         <v>24</v>
       </c>
       <c r="P59" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q59" s="4">
         <v>0</v>
@@ -4004,19 +3994,19 @@
         <v>18</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H60" s="4"/>
       <c r="I60" s="8" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="J60" s="5"/>
       <c r="K60" s="4" t="s">
@@ -4035,7 +4025,7 @@
         <v>24</v>
       </c>
       <c r="P60" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q60" s="4">
         <v>0</v>
@@ -4053,19 +4043,19 @@
         <v>18</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J61" s="5"/>
       <c r="K61" s="4" t="s">
@@ -4078,13 +4068,13 @@
         <v>25</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O61" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P61" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q61" s="4">
         <v>0</v>
@@ -4102,19 +4092,19 @@
         <v>18</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J62" s="5"/>
       <c r="K62" s="4" t="s">
@@ -4127,13 +4117,13 @@
         <v>25</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O62" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P62" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q62" s="4">
         <v>0</v>
@@ -4151,19 +4141,19 @@
         <v>18</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J63" s="5"/>
       <c r="K63" s="4" t="s">
@@ -4176,13 +4166,13 @@
         <v>25</v>
       </c>
       <c r="N63" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O63" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P63" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q63" s="4">
         <v>0</v>
@@ -4200,19 +4190,19 @@
         <v>18</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J64" s="5"/>
       <c r="K64" s="4" t="s">
@@ -4225,13 +4215,13 @@
         <v>25</v>
       </c>
       <c r="N64" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O64" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P64" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q64" s="4">
         <v>0</v>
@@ -4249,19 +4239,19 @@
         <v>18</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J65" s="5"/>
       <c r="K65" s="4" t="s">
@@ -4274,13 +4264,13 @@
         <v>25</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O65" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P65" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q65" s="4">
         <v>0</v>
@@ -4298,19 +4288,19 @@
         <v>18</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J66" s="5"/>
       <c r="K66" s="4" t="s">
@@ -4323,13 +4313,13 @@
         <v>25</v>
       </c>
       <c r="N66" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O66" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P66" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q66" s="4">
         <v>0</v>
@@ -4347,19 +4337,19 @@
         <v>18</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="4" t="s">
@@ -4372,13 +4362,13 @@
         <v>25</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O67" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P67" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q67" s="4">
         <v>0</v>
@@ -4396,19 +4386,19 @@
         <v>18</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J68" s="5"/>
       <c r="K68" s="4" t="s">
@@ -4421,13 +4411,13 @@
         <v>25</v>
       </c>
       <c r="N68" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O68" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P68" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="Q68" s="4">
         <v>0</v>
@@ -4445,10 +4435,10 @@
         <v>18</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
@@ -4457,7 +4447,7 @@
       </c>
       <c r="H69" s="9"/>
       <c r="I69" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="9" t="s">
@@ -4470,7 +4460,7 @@
         <v>25</v>
       </c>
       <c r="N69" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O69" s="9">
         <v>0</v>
@@ -4494,10 +4484,10 @@
         <v>18</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -4506,7 +4496,7 @@
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J70" s="5"/>
       <c r="K70" s="4" t="s">
@@ -4519,7 +4509,7 @@
         <v>25</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O70" s="4">
         <v>0</v>
@@ -4543,10 +4533,10 @@
         <v>18</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -4555,7 +4545,7 @@
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J71" s="5"/>
       <c r="K71" s="4" t="s">
@@ -4568,7 +4558,7 @@
         <v>25</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O71" s="4">
         <v>0</v>
@@ -4592,10 +4582,10 @@
         <v>18</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -4604,7 +4594,7 @@
       </c>
       <c r="H72" s="4"/>
       <c r="I72" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J72" s="5"/>
       <c r="K72" s="4" t="s">
@@ -4617,7 +4607,7 @@
         <v>25</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O72" s="4">
         <v>0</v>
@@ -4641,10 +4631,10 @@
         <v>18</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -4653,7 +4643,7 @@
       </c>
       <c r="H73" s="4"/>
       <c r="I73" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J73" s="5"/>
       <c r="K73" s="4" t="s">
@@ -4666,7 +4656,7 @@
         <v>25</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="O73" s="4">
         <v>0</v>
@@ -4690,10 +4680,10 @@
         <v>18</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
@@ -4702,7 +4692,7 @@
       </c>
       <c r="H74" s="4"/>
       <c r="I74" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J74" s="5"/>
       <c r="K74" s="4" t="s">
@@ -4715,7 +4705,7 @@
         <v>25</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="O74" s="4">
         <v>0</v>
@@ -4736,14 +4726,14 @@
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J75" s="5"/>
       <c r="K75" s="4" t="s">
@@ -4756,7 +4746,7 @@
         <v>25</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O75" s="4">
         <v>0</v>
@@ -4780,10 +4770,10 @@
         <v>18</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
@@ -4792,7 +4782,7 @@
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J76" s="5"/>
       <c r="K76" s="4" t="s">
@@ -4805,7 +4795,7 @@
         <v>25</v>
       </c>
       <c r="N76" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="O76" s="4">
         <v>0</v>
@@ -4829,10 +4819,10 @@
         <v>18</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
@@ -4841,7 +4831,7 @@
       </c>
       <c r="H77" s="7"/>
       <c r="I77" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J77" s="5"/>
       <c r="K77" s="7" t="s">
@@ -4854,7 +4844,7 @@
         <v>25</v>
       </c>
       <c r="N77" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="O77" s="7">
         <v>0</v>
@@ -4878,10 +4868,10 @@
         <v>18</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -4890,7 +4880,7 @@
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J78" s="5"/>
       <c r="K78" s="4" t="s">
@@ -4903,7 +4893,7 @@
         <v>25</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O78" s="4">
         <v>0</v>
@@ -4927,19 +4917,19 @@
         <v>18</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
       <c r="G79" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H79" s="7"/>
       <c r="I79" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J79" s="5"/>
       <c r="K79" s="7" t="s">
@@ -4952,7 +4942,7 @@
         <v>25</v>
       </c>
       <c r="N79" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O79" s="7">
         <v>0</v>
@@ -4976,19 +4966,19 @@
         <v>18</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H80" s="7"/>
       <c r="I80" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J80" s="5"/>
       <c r="K80" s="7" t="s">
@@ -5001,7 +4991,7 @@
         <v>25</v>
       </c>
       <c r="N80" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="O80" s="7">
         <v>0</v>
@@ -5025,13 +5015,13 @@
         <v>18</v>
       </c>
       <c r="C81" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E81" s="12" t="s">
         <v>141</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>143</v>
       </c>
       <c r="F81" s="12"/>
       <c r="G81" s="12"/>
@@ -5048,7 +5038,7 @@
         <v>25</v>
       </c>
       <c r="N81" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O81" s="12">
         <v>0</v>
@@ -5060,7 +5050,7 @@
         <v>0</v>
       </c>
       <c r="R81" s="12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:18" ht="68" x14ac:dyDescent="0.2">
@@ -5071,10 +5061,10 @@
         <v>18</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E82" s="12"/>
       <c r="F82" s="12"/>
@@ -5092,7 +5082,7 @@
         <v>25</v>
       </c>
       <c r="N82" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O82" s="12">
         <v>0</v>
@@ -5104,7 +5094,7 @@
         <v>0</v>
       </c>
       <c r="R82" s="12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -5115,10 +5105,10 @@
         <v>18</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E83" s="12"/>
       <c r="F83" s="12"/>
@@ -5136,7 +5126,7 @@
         <v>25</v>
       </c>
       <c r="N83" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O83" s="12">
         <v>0</v>
@@ -5148,7 +5138,7 @@
         <v>0</v>
       </c>
       <c r="R83" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -5159,17 +5149,17 @@
         <v>18</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J84" s="5"/>
       <c r="K84" s="4" t="s">
@@ -5179,7 +5169,7 @@
         <v>24</v>
       </c>
       <c r="M84" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N84" s="6" t="s">
         <v>28</v>
@@ -5206,17 +5196,17 @@
         <v>18</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
       <c r="I85" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J85" s="5"/>
       <c r="K85" s="4" t="s">
@@ -5226,7 +5216,7 @@
         <v>24</v>
       </c>
       <c r="M85" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N85" s="6" t="s">
         <v>32</v>
@@ -5253,17 +5243,17 @@
         <v>18</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J86" s="5"/>
       <c r="K86" s="4" t="s">
@@ -5273,7 +5263,7 @@
         <v>24</v>
       </c>
       <c r="M86" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N86" s="6" t="s">
         <v>34</v>
@@ -5300,17 +5290,17 @@
         <v>18</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J87" s="5"/>
       <c r="K87" s="4" t="s">
@@ -5320,10 +5310,10 @@
         <v>24</v>
       </c>
       <c r="M87" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N87" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O87" s="4">
         <v>0</v>
@@ -5347,17 +5337,17 @@
         <v>18</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J88" s="5"/>
       <c r="K88" s="4" t="s">
@@ -5367,10 +5357,10 @@
         <v>24</v>
       </c>
       <c r="M88" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O88" s="4">
         <v>0</v>
@@ -5394,17 +5384,17 @@
         <v>18</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J89" s="5"/>
       <c r="K89" s="4" t="s">
@@ -5414,10 +5404,10 @@
         <v>24</v>
       </c>
       <c r="M89" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O89" s="4">
         <v>0</v>
@@ -5441,17 +5431,17 @@
         <v>18</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J90" s="5"/>
       <c r="K90" s="4" t="s">
@@ -5461,10 +5451,10 @@
         <v>24</v>
       </c>
       <c r="M90" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O90" s="4">
         <v>0</v>
@@ -5488,17 +5478,17 @@
         <v>18</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J91" s="5"/>
       <c r="K91" s="4" t="s">
@@ -5508,10 +5498,10 @@
         <v>24</v>
       </c>
       <c r="M91" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N91" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O91" s="4">
         <v>0</v>
@@ -5535,17 +5525,17 @@
         <v>18</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J92" s="5"/>
       <c r="K92" s="4" t="s">
@@ -5555,10 +5545,10 @@
         <v>24</v>
       </c>
       <c r="M92" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N92" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O92" s="4">
         <v>0</v>
@@ -5582,17 +5572,17 @@
         <v>18</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J93" s="5"/>
       <c r="K93" s="4" t="s">
@@ -5602,10 +5592,10 @@
         <v>24</v>
       </c>
       <c r="M93" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N93" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O93" s="4">
         <v>0</v>

</xml_diff>